<commit_message>
Minor updates to terminal sizing and flag settings
</commit_message>
<xml_diff>
--- a/test_files/validation/debug_book.xlsx
+++ b/test_files/validation/debug_book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan Munro\Dropbox\dev\lazarus\computing\z80\box80\test_files\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8619A58-18AE-44E9-A48F-7E7562484986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE902F3-9531-4D4F-B70F-D7EC45776919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="20076" windowHeight="11472" xr2:uid="{84EB85F7-8048-4063-BC53-51767C72ED03}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="20076" windowHeight="11472" xr2:uid="{84EB85F7-8048-4063-BC53-51767C72ED03}"/>
   </bookViews>
   <sheets>
     <sheet name="Compliance" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Mem IY  IX  HL  DE  BC  F A SP</t>
   </si>
@@ -99,12 +99,6 @@
     <t>AND instruction wasn't clearing N flag</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>_ _ _ _ _ _ _ C</t>
-  </si>
-  <si>
     <t>NEG not setting flags correctly</t>
   </si>
   <si>
@@ -138,28 +132,40 @@
     <t>CCF now resets H,N flips C everything else left alone</t>
   </si>
   <si>
-    <t>4121FA09601D59A55B8D7990009A9D29</t>
-  </si>
-  <si>
-    <t>4121FA09601D59A55B8D799094A09D29</t>
-  </si>
-  <si>
-    <t>4121FA09601D59A55B8D799055009D29</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>94</t>
-  </si>
-  <si>
-    <t>A: 9A -&gt; 00</t>
-  </si>
-  <si>
-    <t>_ Z _ H _ P _ C</t>
-  </si>
-  <si>
-    <t>S _ _ H _ P _ _</t>
+    <t>Wanted</t>
+  </si>
+  <si>
+    <t>We got</t>
+  </si>
+  <si>
+    <t>4121FA09601D59A55B8D7990020A9D29</t>
+  </si>
+  <si>
+    <t>4121FA09601D59A55B8D799002049D29</t>
+  </si>
+  <si>
+    <t>4121FA09601D59A55B8D7990060A9D29</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>_ _ _ _ _ _ N _</t>
+  </si>
+  <si>
+    <t>_ _ _ _ _ P N _</t>
+  </si>
+  <si>
+    <t>A: 0A -&gt; 0A</t>
+  </si>
+  <si>
+    <t>A: 0A -&gt; 04</t>
+  </si>
+  <si>
+    <t>Remaining DAA problems, Z180 delivering odd results</t>
   </si>
 </sst>
 </file>
@@ -771,7 +777,7 @@
         <v>0.44888433981576253</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -793,7 +799,7 @@
         <v>0.58532241555783004</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -815,7 +821,7 @@
         <v>0.59901740020470828</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -837,7 +843,7 @@
         <v>0.62661207778915051</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -859,7 +865,7 @@
         <v>0.75238485158648927</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -881,7 +887,7 @@
         <v>0.79430910951893552</v>
       </c>
       <c r="F16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -903,7 +909,7 @@
         <v>0.79430910951893552</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -925,7 +931,7 @@
         <v>0.79430910951893552</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -947,7 +953,7 @@
         <v>0.87815762538382802</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -967,6 +973,9 @@
       <c r="E20" s="10">
         <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
         <v>0.91477993858751283</v>
+      </c>
+      <c r="F20" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -982,7 +991,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1008,7 +1017,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -1017,15 +1026,15 @@
         <v>33</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -1034,7 +1043,7 @@
         <v>35</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>39</v>
@@ -1049,19 +1058,27 @@
         <v>34</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updates to documentation / logs
</commit_message>
<xml_diff>
--- a/test_files/validation/debug_book.xlsx
+++ b/test_files/validation/debug_book.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan Munro\Dropbox\dev\lazarus\computing\z80\box80\test_files\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8619A58-18AE-44E9-A48F-7E7562484986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6E2F30-FDCA-4D51-9E6E-86BB516045EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="20076" windowHeight="11472" xr2:uid="{84EB85F7-8048-4063-BC53-51767C72ED03}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="20076" windowHeight="11472" activeTab="1" xr2:uid="{84EB85F7-8048-4063-BC53-51767C72ED03}"/>
   </bookViews>
   <sheets>
     <sheet name="Compliance" sheetId="2" r:id="rId1"/>
-    <sheet name="Worksheet" sheetId="1" r:id="rId2"/>
+    <sheet name="Tests" sheetId="3" r:id="rId2"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,8 +37,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Duncan Munro</author>
+  </authors>
+  <commentList>
+    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{E23E6411-98CA-4378-8827-6FBB024BD48C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Duncan Munro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Was box80 crash, now OK</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="185">
   <si>
     <t>Mem IY  IX  HL  DE  BC  F A SP</t>
   </si>
@@ -160,6 +195,438 @@
   </si>
   <si>
     <t>S _ _ H _ P _ _</t>
+  </si>
+  <si>
+    <t>ZEXDOC tests being carried out</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>Increment</t>
+  </si>
+  <si>
+    <t>Shift</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Z180</t>
+  </si>
+  <si>
+    <t>box80</t>
+  </si>
+  <si>
+    <t>adc16</t>
+  </si>
+  <si>
+    <t>add16</t>
+  </si>
+  <si>
+    <t>add16x</t>
+  </si>
+  <si>
+    <t>add16y</t>
+  </si>
+  <si>
+    <t>alu8i</t>
+  </si>
+  <si>
+    <t>alu8r</t>
+  </si>
+  <si>
+    <t>alu8rx</t>
+  </si>
+  <si>
+    <t>alu8x</t>
+  </si>
+  <si>
+    <t>bitx</t>
+  </si>
+  <si>
+    <t>bitz80</t>
+  </si>
+  <si>
+    <t>cpd1</t>
+  </si>
+  <si>
+    <t>cpi1</t>
+  </si>
+  <si>
+    <t>daax</t>
+  </si>
+  <si>
+    <t>inca</t>
+  </si>
+  <si>
+    <t>incb</t>
+  </si>
+  <si>
+    <t>incbc</t>
+  </si>
+  <si>
+    <t>incc</t>
+  </si>
+  <si>
+    <t>incd</t>
+  </si>
+  <si>
+    <t>incde</t>
+  </si>
+  <si>
+    <t>ince</t>
+  </si>
+  <si>
+    <t>inch</t>
+  </si>
+  <si>
+    <t>inchl</t>
+  </si>
+  <si>
+    <t>incix</t>
+  </si>
+  <si>
+    <t>inciy</t>
+  </si>
+  <si>
+    <t>incl</t>
+  </si>
+  <si>
+    <t>incm</t>
+  </si>
+  <si>
+    <t>incsp</t>
+  </si>
+  <si>
+    <t>incx</t>
+  </si>
+  <si>
+    <t>incxh</t>
+  </si>
+  <si>
+    <t>incxl</t>
+  </si>
+  <si>
+    <t>incyh</t>
+  </si>
+  <si>
+    <t>incyl</t>
+  </si>
+  <si>
+    <t>ld161</t>
+  </si>
+  <si>
+    <t>ld162</t>
+  </si>
+  <si>
+    <t>ld163</t>
+  </si>
+  <si>
+    <t>ld164</t>
+  </si>
+  <si>
+    <t>ld165</t>
+  </si>
+  <si>
+    <t>ld166</t>
+  </si>
+  <si>
+    <t>ld167</t>
+  </si>
+  <si>
+    <t>ld168</t>
+  </si>
+  <si>
+    <t>ld16im</t>
+  </si>
+  <si>
+    <t>ld16ix</t>
+  </si>
+  <si>
+    <t>ld8bd</t>
+  </si>
+  <si>
+    <t>ld8im</t>
+  </si>
+  <si>
+    <t>ld8imx</t>
+  </si>
+  <si>
+    <t>ld8ix1</t>
+  </si>
+  <si>
+    <t>ld8ix2</t>
+  </si>
+  <si>
+    <t>ld8ix3</t>
+  </si>
+  <si>
+    <t>ld8ixy</t>
+  </si>
+  <si>
+    <t>ld8rr</t>
+  </si>
+  <si>
+    <t>ld8rrx</t>
+  </si>
+  <si>
+    <t>lda</t>
+  </si>
+  <si>
+    <t>ldd1</t>
+  </si>
+  <si>
+    <t>ldd2</t>
+  </si>
+  <si>
+    <t>ldi1</t>
+  </si>
+  <si>
+    <t>ldi2</t>
+  </si>
+  <si>
+    <t>negx</t>
+  </si>
+  <si>
+    <t>rldx</t>
+  </si>
+  <si>
+    <t>rot8080</t>
+  </si>
+  <si>
+    <t>rotxy</t>
+  </si>
+  <si>
+    <t>srz80</t>
+  </si>
+  <si>
+    <t>srzx</t>
+  </si>
+  <si>
+    <t>st8ix1</t>
+  </si>
+  <si>
+    <t>st8ix2</t>
+  </si>
+  <si>
+    <t>st8ix3</t>
+  </si>
+  <si>
+    <t>stabd</t>
+  </si>
+  <si>
+    <t>&lt;adc,sbc&gt; hl,&lt;bc,de,hl,sp&gt;</t>
+  </si>
+  <si>
+    <t>add hl,&lt;bc,de,hl,sp&gt;</t>
+  </si>
+  <si>
+    <t>add ix,&lt;bc,de,ix,sp&gt;</t>
+  </si>
+  <si>
+    <t>add iy,&lt;bc,de,iy,sp&gt;</t>
+  </si>
+  <si>
+    <t>aluop a,nn</t>
+  </si>
+  <si>
+    <t>aluop a,&lt;b,c,d,e,h,l,(hl),a&gt;</t>
+  </si>
+  <si>
+    <t>aluop a,&lt;ixh,ixl,iyh,iyl&gt;</t>
+  </si>
+  <si>
+    <t>aluop a,(&lt;ix,iy&gt;+1)</t>
+  </si>
+  <si>
+    <t>bit n,(&lt;ix,iy&gt;+1)</t>
+  </si>
+  <si>
+    <t>bit n,&lt;b,c,d,e,h,l,(hl),a&gt;</t>
+  </si>
+  <si>
+    <t>cpd&lt;r&gt;</t>
+  </si>
+  <si>
+    <t>cpi&lt;r&gt;</t>
+  </si>
+  <si>
+    <t>&lt;daa,cpl,scf,ccf&gt;</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; a</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; b</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; bc</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; c</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; d</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; de</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; e</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; h</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; hl</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; ix</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; iy</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; l</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; (hl)</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; sp</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; (&lt;ix,iy&gt;+1)</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; ixh</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; ixl</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; iyh</t>
+  </si>
+  <si>
+    <t>&lt;inc,dec&gt; iyl</t>
+  </si>
+  <si>
+    <t>ld &lt;bc,de&gt;,(nnnn)</t>
+  </si>
+  <si>
+    <t>ld hl,(nnnn)</t>
+  </si>
+  <si>
+    <t>ld sp,(nnnn)</t>
+  </si>
+  <si>
+    <t>ld &lt;ix,iy&gt;,(nnnn)</t>
+  </si>
+  <si>
+    <t>ld (nnnn),&lt;bc,de&gt;</t>
+  </si>
+  <si>
+    <t>ld (nnnn),hl</t>
+  </si>
+  <si>
+    <t>ld (nnnn),sp</t>
+  </si>
+  <si>
+    <t>ld (nnnn),&lt;ix,iy&gt;</t>
+  </si>
+  <si>
+    <t>ld &lt;bc,de,hl,sp&gt;,nnnn</t>
+  </si>
+  <si>
+    <t>ld &lt;ix,iy&gt;,nnnn</t>
+  </si>
+  <si>
+    <t>ld a,&lt;(bc),(de)&gt;</t>
+  </si>
+  <si>
+    <t>ld &lt;b,c,d,e,h,l,(hl),a&gt;,nn</t>
+  </si>
+  <si>
+    <t>ld (&lt;ix,iy&gt;+1),nn</t>
+  </si>
+  <si>
+    <t>ld &lt;b,c,d,e&gt;,(&lt;ix,iy&gt;+1)</t>
+  </si>
+  <si>
+    <t>ld &lt;h,l&gt;,(&lt;ix,iy&gt;+1)</t>
+  </si>
+  <si>
+    <t>ld a,(&lt;ix,iy&gt;+1)</t>
+  </si>
+  <si>
+    <t>ld &lt;ixh,ixl,iyh,iyl&gt;,nn</t>
+  </si>
+  <si>
+    <t>ld &lt;bcdehla&gt;,&lt;bcdehla&gt;</t>
+  </si>
+  <si>
+    <t>ld &lt;bcdexya&gt;,&lt;bcdexya&gt;</t>
+  </si>
+  <si>
+    <t>ld a,(nnnn) / ld (nnnn),a</t>
+  </si>
+  <si>
+    <t>ldd&lt;r&gt; (1)</t>
+  </si>
+  <si>
+    <t>ldd&lt;r&gt; (2)</t>
+  </si>
+  <si>
+    <t>ldi&lt;r&gt; (1)</t>
+  </si>
+  <si>
+    <t>ldi&lt;r&gt; (2)</t>
+  </si>
+  <si>
+    <t>neg</t>
+  </si>
+  <si>
+    <t>&lt;rrd,rld&gt;</t>
+  </si>
+  <si>
+    <t>&lt;rlca,rrca,rla,rra&gt;</t>
+  </si>
+  <si>
+    <t>shf/rot (&lt;ix,iy&gt;+1)</t>
+  </si>
+  <si>
+    <t>rotz80</t>
+  </si>
+  <si>
+    <t>shf/rot &lt;b,c,d,e,h,l,(hl),a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;set,res&gt; n,&lt;bcdehl(hl)a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;set,res&gt; n,(&lt;ix,iy&gt;+1)</t>
+  </si>
+  <si>
+    <t>ld (&lt;ix,iy&gt;+1),&lt;b,c,d,e&gt;</t>
+  </si>
+  <si>
+    <t>ld (&lt;ix,iy&gt;+1),&lt;h,l&gt;</t>
+  </si>
+  <si>
+    <t>ld (&lt;ix,iy&gt;+1),a</t>
+  </si>
+  <si>
+    <t>ld (&lt;bc,de&gt;),a</t>
+  </si>
+  <si>
+    <t>Crash</t>
+  </si>
+  <si>
+    <t>b80 crash</t>
   </si>
 </sst>
 </file>
@@ -172,7 +639,7 @@
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,6 +668,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -224,7 +712,7 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -246,13 +734,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -301,17 +801,35 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CCD46394-3C59-49D5-A3BE-54484FCE77F1}" name="Table1" displayName="Table1" ref="A6:F20" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CCD46394-3C59-49D5-A3BE-54484FCE77F1}" name="Table1" displayName="Table1" ref="A6:F20" totalsRowShown="0" headerRowDxfId="8">
   <autoFilter ref="A6:F20" xr:uid="{CCD46394-3C59-49D5-A3BE-54484FCE77F1}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{645467FE-6092-4669-8C66-53405E1B316C}" name="Date/Tim" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{0FDF52E0-80D4-44BC-BCD2-1F61AB42DBEC}" name="Tests     " dataDxfId="3" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{CD4822BD-2D77-4251-B2FA-BAA7F3F078D0}" name="Failures     " dataDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="4" xr3:uid="{F6F4EA73-6E79-45BC-BD70-1D4E8E6DCC01}" name="%     " dataDxfId="1" dataCellStyle="Percent">
+    <tableColumn id="1" xr3:uid="{645467FE-6092-4669-8C66-53405E1B316C}" name="Date/Tim" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{0FDF52E0-80D4-44BC-BCD2-1F61AB42DBEC}" name="Tests     " dataDxfId="6" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{CD4822BD-2D77-4251-B2FA-BAA7F3F078D0}" name="Failures     " dataDxfId="5" dataCellStyle="Comma"/>
+    <tableColumn id="4" xr3:uid="{F6F4EA73-6E79-45BC-BD70-1D4E8E6DCC01}" name="%     " dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{2425AE14-49B5-4673-8753-20CA04B4D2C1}" name="Clearup     " dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="6" xr3:uid="{2425AE14-49B5-4673-8753-20CA04B4D2C1}" name="Clearup     " dataDxfId="3" dataCellStyle="Percent"/>
     <tableColumn id="5" xr3:uid="{37488288-AF62-4EAB-9CD0-9B24229D85F2}" name="Notable fixes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{34B62E41-2298-4210-8966-65874EBDA708}" name="Table2" displayName="Table2" ref="A4:G72" totalsRowCount="1" headerRowDxfId="1">
+  <autoFilter ref="A4:G71" xr:uid="{34B62E41-2298-4210-8966-65874EBDA708}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{395A6183-A6BB-4FE0-816C-3055C429C150}" name="Name" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{B3832540-120B-4C79-AB63-366F384FFC96}" name="Instructions"/>
+    <tableColumn id="3" xr3:uid="{1BD17A57-95F7-426C-894B-906B13DE9059}" name="Increment"/>
+    <tableColumn id="4" xr3:uid="{B75C55FD-5323-46D9-9783-F61A4828C082}" name="Shift"/>
+    <tableColumn id="5" xr3:uid="{C9B3CC2C-1370-460A-B8D4-2B8E921CD89E}" name="Total" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="0">
+      <calculatedColumnFormula>C5*D5</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{2C15C62B-3C34-4879-9300-FEDEB15F1D58}" name="Z180"/>
+    <tableColumn id="7" xr3:uid="{E617E5B1-6B4E-40F0-BC9A-62C280715120}" name="box80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -616,9 +1134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D7535A-9EF6-43CB-A66F-D74C02DC0D46}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -978,6 +1494,1336 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D38BA54-A9BA-4382-B8C9-AD0F8112E2CF}">
+  <dimension ref="A1:G72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5">
+        <v>1024</v>
+      </c>
+      <c r="D5">
+        <v>38</v>
+      </c>
+      <c r="E5" s="12">
+        <f>C5*D5</f>
+        <v>38912</v>
+      </c>
+      <c r="G5" s="13">
+        <v>45123</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6">
+        <v>512</v>
+      </c>
+      <c r="D6">
+        <v>38</v>
+      </c>
+      <c r="E6" s="12">
+        <f t="shared" ref="E6:E69" si="0">C6*D6</f>
+        <v>19456</v>
+      </c>
+      <c r="G6" s="13">
+        <v>45123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7">
+        <v>512</v>
+      </c>
+      <c r="D7">
+        <v>38</v>
+      </c>
+      <c r="E7" s="12">
+        <f t="shared" si="0"/>
+        <v>19456</v>
+      </c>
+      <c r="G7" s="13">
+        <v>45123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8">
+        <v>512</v>
+      </c>
+      <c r="D8">
+        <v>38</v>
+      </c>
+      <c r="E8" s="12">
+        <f t="shared" si="0"/>
+        <v>19456</v>
+      </c>
+      <c r="G8" s="13">
+        <v>45123</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9">
+        <v>2048</v>
+      </c>
+      <c r="D9">
+        <v>14</v>
+      </c>
+      <c r="E9" s="12">
+        <f t="shared" si="0"/>
+        <v>28672</v>
+      </c>
+      <c r="G9" s="13">
+        <v>45123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="12">
+        <v>16384</v>
+      </c>
+      <c r="D10">
+        <v>46</v>
+      </c>
+      <c r="E10" s="12">
+        <f t="shared" si="0"/>
+        <v>753664</v>
+      </c>
+      <c r="G10" s="13">
+        <v>45123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="12">
+        <v>8192</v>
+      </c>
+      <c r="D11">
+        <v>46</v>
+      </c>
+      <c r="E11" s="12">
+        <f t="shared" si="0"/>
+        <v>376832</v>
+      </c>
+      <c r="F11" t="s">
+        <v>183</v>
+      </c>
+      <c r="G11" s="13">
+        <v>45123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" t="s">
+        <v>122</v>
+      </c>
+      <c r="C12" s="12">
+        <v>16384</v>
+      </c>
+      <c r="D12">
+        <v>14</v>
+      </c>
+      <c r="E12" s="12">
+        <f t="shared" si="0"/>
+        <v>229376</v>
+      </c>
+      <c r="G12" s="13">
+        <v>45123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s">
+        <v>123</v>
+      </c>
+      <c r="C13">
+        <v>256</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13" s="12">
+        <f t="shared" si="0"/>
+        <v>2048</v>
+      </c>
+      <c r="G13" s="13">
+        <v>45123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14">
+        <v>1024</v>
+      </c>
+      <c r="D14">
+        <v>48</v>
+      </c>
+      <c r="E14" s="12">
+        <f t="shared" si="0"/>
+        <v>49152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15">
+        <v>1024</v>
+      </c>
+      <c r="D15">
+        <v>6</v>
+      </c>
+      <c r="E15" s="12">
+        <f t="shared" si="0"/>
+        <v>6144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B16" t="s">
+        <v>126</v>
+      </c>
+      <c r="C16">
+        <v>1024</v>
+      </c>
+      <c r="D16">
+        <v>6</v>
+      </c>
+      <c r="E16" s="12">
+        <f t="shared" si="0"/>
+        <v>6144</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" t="s">
+        <v>127</v>
+      </c>
+      <c r="C17" s="12">
+        <v>65536</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="12">
+        <f t="shared" si="0"/>
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18">
+        <v>512</v>
+      </c>
+      <c r="D18">
+        <v>6</v>
+      </c>
+      <c r="E18" s="12">
+        <f t="shared" si="0"/>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>129</v>
+      </c>
+      <c r="C19">
+        <v>512</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19" s="12">
+        <f t="shared" si="0"/>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" t="s">
+        <v>130</v>
+      </c>
+      <c r="C20">
+        <v>256</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20" s="12">
+        <f t="shared" si="0"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>65</v>
+      </c>
+      <c r="B21" t="s">
+        <v>131</v>
+      </c>
+      <c r="C21">
+        <v>512</v>
+      </c>
+      <c r="D21">
+        <v>6</v>
+      </c>
+      <c r="E21" s="12">
+        <f t="shared" si="0"/>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22">
+        <v>512</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22" s="12">
+        <f t="shared" si="0"/>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23">
+        <v>256</v>
+      </c>
+      <c r="D23">
+        <v>6</v>
+      </c>
+      <c r="E23" s="12">
+        <f t="shared" si="0"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24">
+        <v>512</v>
+      </c>
+      <c r="D24">
+        <v>6</v>
+      </c>
+      <c r="E24" s="12">
+        <f t="shared" si="0"/>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25">
+        <v>512</v>
+      </c>
+      <c r="D25">
+        <v>6</v>
+      </c>
+      <c r="E25" s="12">
+        <f t="shared" si="0"/>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26">
+        <v>256</v>
+      </c>
+      <c r="D26">
+        <v>6</v>
+      </c>
+      <c r="E26" s="12">
+        <f t="shared" si="0"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27">
+        <v>256</v>
+      </c>
+      <c r="D27">
+        <v>6</v>
+      </c>
+      <c r="E27" s="12">
+        <f t="shared" si="0"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C28">
+        <v>256</v>
+      </c>
+      <c r="D28">
+        <v>6</v>
+      </c>
+      <c r="E28" s="12">
+        <f t="shared" si="0"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29">
+        <v>512</v>
+      </c>
+      <c r="D29">
+        <v>6</v>
+      </c>
+      <c r="E29" s="12">
+        <f t="shared" si="0"/>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30">
+        <v>512</v>
+      </c>
+      <c r="D30">
+        <v>6</v>
+      </c>
+      <c r="E30" s="12">
+        <f t="shared" si="0"/>
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s">
+        <v>141</v>
+      </c>
+      <c r="C31">
+        <v>256</v>
+      </c>
+      <c r="D31">
+        <v>6</v>
+      </c>
+      <c r="E31" s="12">
+        <f t="shared" si="0"/>
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32">
+        <v>1024</v>
+      </c>
+      <c r="D32">
+        <v>6</v>
+      </c>
+      <c r="E32" s="12">
+        <f t="shared" si="0"/>
+        <v>6144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" t="s">
+        <v>143</v>
+      </c>
+      <c r="C33">
+        <v>512</v>
+      </c>
+      <c r="D33">
+        <v>6</v>
+      </c>
+      <c r="E33" s="12">
+        <f t="shared" si="0"/>
+        <v>3072</v>
+      </c>
+      <c r="F33" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="B34" t="s">
+        <v>144</v>
+      </c>
+      <c r="C34">
+        <v>512</v>
+      </c>
+      <c r="D34">
+        <v>6</v>
+      </c>
+      <c r="E34" s="12">
+        <f t="shared" si="0"/>
+        <v>3072</v>
+      </c>
+      <c r="F34" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35">
+        <v>512</v>
+      </c>
+      <c r="D35">
+        <v>6</v>
+      </c>
+      <c r="E35" s="12">
+        <f t="shared" si="0"/>
+        <v>3072</v>
+      </c>
+      <c r="F35" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>80</v>
+      </c>
+      <c r="B36" t="s">
+        <v>146</v>
+      </c>
+      <c r="C36">
+        <v>512</v>
+      </c>
+      <c r="D36">
+        <v>6</v>
+      </c>
+      <c r="E36" s="12">
+        <f t="shared" si="0"/>
+        <v>3072</v>
+      </c>
+      <c r="F36" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>81</v>
+      </c>
+      <c r="B37" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>16</v>
+      </c>
+      <c r="E37" s="12">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" t="s">
+        <v>148</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38">
+        <v>16</v>
+      </c>
+      <c r="E38" s="12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>83</v>
+      </c>
+      <c r="B39" t="s">
+        <v>149</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>16</v>
+      </c>
+      <c r="E39" s="12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <v>16</v>
+      </c>
+      <c r="E40" s="12">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" t="s">
+        <v>151</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41">
+        <v>32</v>
+      </c>
+      <c r="E41" s="12">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>16</v>
+      </c>
+      <c r="E42" s="12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" t="s">
+        <v>153</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>16</v>
+      </c>
+      <c r="E43" s="12">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>32</v>
+      </c>
+      <c r="E44" s="12">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" t="s">
+        <v>155</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>16</v>
+      </c>
+      <c r="E45" s="12">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
+        <v>156</v>
+      </c>
+      <c r="C46">
+        <v>2</v>
+      </c>
+      <c r="D46">
+        <v>16</v>
+      </c>
+      <c r="E46" s="12">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47" t="s">
+        <v>157</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>22</v>
+      </c>
+      <c r="E47" s="12">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" t="s">
+        <v>158</v>
+      </c>
+      <c r="C48">
+        <v>8</v>
+      </c>
+      <c r="D48">
+        <v>8</v>
+      </c>
+      <c r="E48" s="12">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>93</v>
+      </c>
+      <c r="B49" t="s">
+        <v>159</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>16</v>
+      </c>
+      <c r="E49" s="12">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>94</v>
+      </c>
+      <c r="B50" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50">
+        <v>32</v>
+      </c>
+      <c r="D50">
+        <v>16</v>
+      </c>
+      <c r="E50" s="12">
+        <f t="shared" si="0"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51">
+        <v>16</v>
+      </c>
+      <c r="D51">
+        <v>16</v>
+      </c>
+      <c r="E51" s="12">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" t="s">
+        <v>162</v>
+      </c>
+      <c r="C52">
+        <v>8</v>
+      </c>
+      <c r="D52">
+        <v>16</v>
+      </c>
+      <c r="E52" s="12">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" t="s">
+        <v>163</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+      <c r="D53">
+        <v>8</v>
+      </c>
+      <c r="E53" s="12">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="F53" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" t="s">
+        <v>164</v>
+      </c>
+      <c r="C54">
+        <v>64</v>
+      </c>
+      <c r="D54">
+        <v>54</v>
+      </c>
+      <c r="E54" s="12">
+        <f t="shared" si="0"/>
+        <v>3456</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>99</v>
+      </c>
+      <c r="B55" t="s">
+        <v>165</v>
+      </c>
+      <c r="C55">
+        <v>128</v>
+      </c>
+      <c r="D55">
+        <v>54</v>
+      </c>
+      <c r="E55" s="12">
+        <f t="shared" si="0"/>
+        <v>6912</v>
+      </c>
+      <c r="F55" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>100</v>
+      </c>
+      <c r="B56" t="s">
+        <v>166</v>
+      </c>
+      <c r="C56">
+        <v>2</v>
+      </c>
+      <c r="D56">
+        <v>22</v>
+      </c>
+      <c r="E56" s="12">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" t="s">
+        <v>167</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>22</v>
+      </c>
+      <c r="E57" s="12">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>102</v>
+      </c>
+      <c r="B58" t="s">
+        <v>168</v>
+      </c>
+      <c r="C58">
+        <v>2</v>
+      </c>
+      <c r="D58">
+        <v>22</v>
+      </c>
+      <c r="E58" s="12">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" t="s">
+        <v>169</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59">
+        <v>22</v>
+      </c>
+      <c r="E59" s="12">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>104</v>
+      </c>
+      <c r="B60" t="s">
+        <v>170</v>
+      </c>
+      <c r="C60">
+        <v>2</v>
+      </c>
+      <c r="D60">
+        <v>22</v>
+      </c>
+      <c r="E60" s="12">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" t="s">
+        <v>171</v>
+      </c>
+      <c r="C61" s="12">
+        <v>16384</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61" s="12">
+        <f t="shared" si="0"/>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>106</v>
+      </c>
+      <c r="B62" t="s">
+        <v>172</v>
+      </c>
+      <c r="C62">
+        <v>512</v>
+      </c>
+      <c r="D62">
+        <v>14</v>
+      </c>
+      <c r="E62" s="12">
+        <f t="shared" si="0"/>
+        <v>7168</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" t="s">
+        <v>173</v>
+      </c>
+      <c r="C63">
+        <v>1024</v>
+      </c>
+      <c r="D63">
+        <v>6</v>
+      </c>
+      <c r="E63" s="12">
+        <f t="shared" si="0"/>
+        <v>6144</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>108</v>
+      </c>
+      <c r="B64" t="s">
+        <v>174</v>
+      </c>
+      <c r="C64">
+        <v>32</v>
+      </c>
+      <c r="D64">
+        <v>13</v>
+      </c>
+      <c r="E64" s="12">
+        <f t="shared" si="0"/>
+        <v>416</v>
+      </c>
+      <c r="F64" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>175</v>
+      </c>
+      <c r="B65" t="s">
+        <v>176</v>
+      </c>
+      <c r="C65">
+        <v>128</v>
+      </c>
+      <c r="D65">
+        <v>53</v>
+      </c>
+      <c r="E65" s="12">
+        <f t="shared" si="0"/>
+        <v>6784</v>
+      </c>
+      <c r="F65" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>109</v>
+      </c>
+      <c r="B66" t="s">
+        <v>177</v>
+      </c>
+      <c r="C66">
+        <v>128</v>
+      </c>
+      <c r="D66">
+        <v>62</v>
+      </c>
+      <c r="E66" s="12">
+        <f t="shared" si="0"/>
+        <v>7936</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>110</v>
+      </c>
+      <c r="B67" t="s">
+        <v>178</v>
+      </c>
+      <c r="C67">
+        <v>128</v>
+      </c>
+      <c r="D67">
+        <v>14</v>
+      </c>
+      <c r="E67" s="12">
+        <f t="shared" si="0"/>
+        <v>1792</v>
+      </c>
+      <c r="G67" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>111</v>
+      </c>
+      <c r="B68" t="s">
+        <v>179</v>
+      </c>
+      <c r="C68">
+        <v>32</v>
+      </c>
+      <c r="D68">
+        <v>32</v>
+      </c>
+      <c r="E68" s="12">
+        <f t="shared" si="0"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>112</v>
+      </c>
+      <c r="B69" t="s">
+        <v>180</v>
+      </c>
+      <c r="C69">
+        <v>16</v>
+      </c>
+      <c r="D69">
+        <v>32</v>
+      </c>
+      <c r="E69" s="12">
+        <f t="shared" si="0"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>113</v>
+      </c>
+      <c r="B70" t="s">
+        <v>181</v>
+      </c>
+      <c r="C70">
+        <v>8</v>
+      </c>
+      <c r="D70">
+        <v>8</v>
+      </c>
+      <c r="E70" s="12">
+        <f t="shared" ref="E70:E71" si="1">C70*D70</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>114</v>
+      </c>
+      <c r="B71" t="s">
+        <v>182</v>
+      </c>
+      <c r="C71">
+        <v>4</v>
+      </c>
+      <c r="D71">
+        <v>24</v>
+      </c>
+      <c r="E71" s="12">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>46</v>
+      </c>
+      <c r="E72" s="12">
+        <f>SUBTOTAL(109,Table2[Total])</f>
+        <v>1727400</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD42418-4C6D-4C72-8A5F-6805A050D2F2}">
   <dimension ref="A1:E7"/>
   <sheetViews>

</xml_diff>

<commit_message>
Further changes to instruction processing after running test suite
</commit_message>
<xml_diff>
--- a/test_files/validation/debug_book.xlsx
+++ b/test_files/validation/debug_book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan Munro\Dropbox\dev\lazarus\computing\z80\box80\test_files\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6E2F30-FDCA-4D51-9E6E-86BB516045EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6DD020-A2D3-4AC1-8495-3686367BD5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="732" yWindow="732" windowWidth="20076" windowHeight="11472" activeTab="1" xr2:uid="{84EB85F7-8048-4063-BC53-51767C72ED03}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="200">
   <si>
     <t>Mem IY  IX  HL  DE  BC  F A SP</t>
   </si>
@@ -134,12 +134,6 @@
     <t>AND instruction wasn't clearing N flag</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
-    <t>_ _ _ _ _ _ _ C</t>
-  </si>
-  <si>
     <t>NEG not setting flags correctly</t>
   </si>
   <si>
@@ -158,12 +152,6 @@
     <t>CCF not setting flags correctly</t>
   </si>
   <si>
-    <t>3F</t>
-  </si>
-  <si>
-    <t>CCF</t>
-  </si>
-  <si>
     <t>Further changes to CCF but not effective</t>
   </si>
   <si>
@@ -173,30 +161,6 @@
     <t>CCF now resets H,N flips C everything else left alone</t>
   </si>
   <si>
-    <t>4121FA09601D59A55B8D7990009A9D29</t>
-  </si>
-  <si>
-    <t>4121FA09601D59A55B8D799094A09D29</t>
-  </si>
-  <si>
-    <t>4121FA09601D59A55B8D799055009D29</t>
-  </si>
-  <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>94</t>
-  </si>
-  <si>
-    <t>A: 9A -&gt; 00</t>
-  </si>
-  <si>
-    <t>_ Z _ H _ P _ C</t>
-  </si>
-  <si>
-    <t>S _ _ H _ P _ _</t>
-  </si>
-  <si>
     <t>ZEXDOC tests being carried out</t>
   </si>
   <si>
@@ -627,6 +591,87 @@
   </si>
   <si>
     <t>b80 crash</t>
+  </si>
+  <si>
+    <t>Further tests run which had previously crashed</t>
+  </si>
+  <si>
+    <t>SC131 tests re-run for add hl,&lt;bc,de,hl,sp&gt;</t>
+  </si>
+  <si>
+    <t>Box80 tests re-run for aluop a,&lt;b,c,d,e,h,l,(hl),a&gt;</t>
+  </si>
+  <si>
+    <t>Fixed issues with LD &lt;reg8&gt;,(IX/IY+n)</t>
+  </si>
+  <si>
+    <t>Fixed issues with LD &lt;H,L&gt;,(&lt;IX,IY&gt;+n)</t>
+  </si>
+  <si>
+    <t>Fixed issues with LD (&lt;IX,IY&gt;+n),&lt;reg8&gt;</t>
+  </si>
+  <si>
+    <t>Fixed issues with LD (&lt;IX,IY&gt;+n),A</t>
+  </si>
+  <si>
+    <t>Fixed issues with LD A,(&lt;IX,IY&gt;+n)</t>
+  </si>
+  <si>
+    <t>Box80 tests re-run for aluop a,(&lt;ix,iy&gt;+1)</t>
+  </si>
+  <si>
+    <t>$00</t>
+  </si>
+  <si>
+    <t>$04</t>
+  </si>
+  <si>
+    <t>_ _ _ _ _ _ _ _</t>
+  </si>
+  <si>
+    <t>_ _ _ _ _ P _ _</t>
+  </si>
+  <si>
+    <t>SC131 tests re-run for &lt;rrd,rld&gt;</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Box80 is setting Z flag, Z180 isn't</t>
+  </si>
+  <si>
+    <t>$14</t>
+  </si>
+  <si>
+    <t>_ _ _ H _ P _ _</t>
+  </si>
+  <si>
+    <t>Block move instructions had errors, now fixed</t>
+  </si>
+  <si>
+    <t>$FD $09</t>
+  </si>
+  <si>
+    <t>ADD IY,BC</t>
+  </si>
+  <si>
+    <t>C2C72624C151963EF40F0F51921EEA71</t>
+  </si>
+  <si>
+    <t>C2C73575C151963EC7119EC151963EF4</t>
+  </si>
+  <si>
+    <t>C2C73575C151963EF40F0F51801EEA71</t>
+  </si>
+  <si>
+    <t>$2426 + $510F -&gt; $7535</t>
+  </si>
+  <si>
+    <t>Box80 tests re-run for add iy,&lt;bc,de,iy,sp&gt;</t>
+  </si>
+  <si>
+    <t>Box80 tests re-run for bit n,(&lt;ix,iy&gt;+1)</t>
   </si>
 </sst>
 </file>
@@ -748,10 +793,10 @@
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -801,8 +846,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CCD46394-3C59-49D5-A3BE-54484FCE77F1}" name="Table1" displayName="Table1" ref="A6:F20" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A6:F20" xr:uid="{CCD46394-3C59-49D5-A3BE-54484FCE77F1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CCD46394-3C59-49D5-A3BE-54484FCE77F1}" name="Table1" displayName="Table1" ref="A6:F33" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A6:F33" xr:uid="{CCD46394-3C59-49D5-A3BE-54484FCE77F1}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{645467FE-6092-4669-8C66-53405E1B316C}" name="Date/Tim" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{0FDF52E0-80D4-44BC-BCD2-1F61AB42DBEC}" name="Tests     " dataDxfId="6" dataCellStyle="Comma"/>
@@ -818,18 +863,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{34B62E41-2298-4210-8966-65874EBDA708}" name="Table2" displayName="Table2" ref="A4:G72" totalsRowCount="1" headerRowDxfId="1">
-  <autoFilter ref="A4:G71" xr:uid="{34B62E41-2298-4210-8966-65874EBDA708}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{34B62E41-2298-4210-8966-65874EBDA708}" name="Table2" displayName="Table2" ref="A4:H72" totalsRowCount="1" headerRowDxfId="2">
+  <autoFilter ref="A4:H71" xr:uid="{34B62E41-2298-4210-8966-65874EBDA708}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{395A6183-A6BB-4FE0-816C-3055C429C150}" name="Name" totalsRowLabel="Total"/>
     <tableColumn id="2" xr3:uid="{B3832540-120B-4C79-AB63-366F384FFC96}" name="Instructions"/>
     <tableColumn id="3" xr3:uid="{1BD17A57-95F7-426C-894B-906B13DE9059}" name="Increment"/>
     <tableColumn id="4" xr3:uid="{B75C55FD-5323-46D9-9783-F61A4828C082}" name="Shift"/>
-    <tableColumn id="5" xr3:uid="{C9B3CC2C-1370-460A-B8D4-2B8E921CD89E}" name="Total" totalsRowFunction="sum" dataDxfId="2" totalsRowDxfId="0">
+    <tableColumn id="5" xr3:uid="{C9B3CC2C-1370-460A-B8D4-2B8E921CD89E}" name="Total" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>C5*D5</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{2C15C62B-3C34-4879-9300-FEDEB15F1D58}" name="Z180"/>
     <tableColumn id="7" xr3:uid="{E617E5B1-6B4E-40F0-BC9A-62C280715120}" name="box80"/>
+    <tableColumn id="8" xr3:uid="{1C179648-F801-45C7-9A15-3E5C458BDE19}" name="Notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1132,14 +1178,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D7535A-9EF6-43CB-A66F-D74C02DC0D46}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.88671875" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.109375" customWidth="1"/>
     <col min="6" max="6" width="50.109375" customWidth="1"/>
@@ -1287,7 +1335,7 @@
         <v>0.44888433981576253</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -1309,7 +1357,7 @@
         <v>0.58532241555783004</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -1331,7 +1379,7 @@
         <v>0.59901740020470828</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1353,7 +1401,7 @@
         <v>0.62661207778915051</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1375,7 +1423,7 @@
         <v>0.75238485158648927</v>
       </c>
       <c r="F15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1397,7 +1445,7 @@
         <v>0.79430910951893552</v>
       </c>
       <c r="F16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1419,7 +1467,7 @@
         <v>0.79430910951893552</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1441,7 +1489,7 @@
         <v>0.79430910951893552</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1463,7 +1511,7 @@
         <v>0.87815762538382802</v>
       </c>
       <c r="F19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1483,6 +1531,292 @@
       <c r="E20" s="10">
         <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
         <v>0.91477993858751283</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>45123.414583333331</v>
+      </c>
+      <c r="B21" s="8">
+        <v>2072078</v>
+      </c>
+      <c r="C21" s="8">
+        <v>44377</v>
+      </c>
+      <c r="D21" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>2.1416664816671958E-2</v>
+      </c>
+      <c r="E21" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.54578300921187306</v>
+      </c>
+      <c r="F21" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>45123.436805555553</v>
+      </c>
+      <c r="B22" s="8">
+        <v>2072078</v>
+      </c>
+      <c r="C22" s="8">
+        <v>31961</v>
+      </c>
+      <c r="D22" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>1.5424612393934977E-2</v>
+      </c>
+      <c r="E22" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.67286591606960078</v>
+      </c>
+      <c r="F22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
+        <v>45123.463194444441</v>
+      </c>
+      <c r="B23" s="8">
+        <v>2072078</v>
+      </c>
+      <c r="C23" s="8">
+        <v>31299</v>
+      </c>
+      <c r="D23" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>1.5105126351421133E-2</v>
+      </c>
+      <c r="E23" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.67964176049129987</v>
+      </c>
+      <c r="F23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>45123.472916666666</v>
+      </c>
+      <c r="B24" s="8">
+        <v>2072078</v>
+      </c>
+      <c r="C24" s="8">
+        <v>30756</v>
+      </c>
+      <c r="D24" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>1.4843070579389385E-2</v>
+      </c>
+      <c r="E24" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.68519959058341862</v>
+      </c>
+      <c r="F24" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>45123.491666666669</v>
+      </c>
+      <c r="B25" s="8">
+        <v>2072078</v>
+      </c>
+      <c r="C25" s="8">
+        <v>30485</v>
+      </c>
+      <c r="D25" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>1.4712283997030999E-2</v>
+      </c>
+      <c r="E25" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.68797338792221086</v>
+      </c>
+      <c r="F25" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>45123.504166666666</v>
+      </c>
+      <c r="B26" s="8">
+        <v>2072078</v>
+      </c>
+      <c r="C26" s="8">
+        <v>29159</v>
+      </c>
+      <c r="D26" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>1.4072346697373362E-2</v>
+      </c>
+      <c r="E26" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.70154554759467758</v>
+      </c>
+      <c r="F26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>45123.509027777778</v>
+      </c>
+      <c r="B27" s="8">
+        <v>2072078</v>
+      </c>
+      <c r="C27" s="8">
+        <v>29088</v>
+      </c>
+      <c r="D27" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>1.4038081578010094E-2</v>
+      </c>
+      <c r="E27" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.70227226202661208</v>
+      </c>
+      <c r="F27" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>45123.511805555558</v>
+      </c>
+      <c r="B28" s="8">
+        <v>2072078</v>
+      </c>
+      <c r="C28" s="8">
+        <v>28957</v>
+      </c>
+      <c r="D28" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>1.3974860019748292E-2</v>
+      </c>
+      <c r="E28" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.70361310133060384</v>
+      </c>
+      <c r="F28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
+        <v>45123.519444444442</v>
+      </c>
+      <c r="B29" s="8">
+        <v>2072078</v>
+      </c>
+      <c r="C29" s="8">
+        <v>28909</v>
+      </c>
+      <c r="D29" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>1.3951694868629462E-2</v>
+      </c>
+      <c r="E29" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.7041044012282498</v>
+      </c>
+      <c r="F29" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
+        <v>45123.530555555553</v>
+      </c>
+      <c r="B30" s="8">
+        <v>2072078</v>
+      </c>
+      <c r="C30" s="8">
+        <v>28909</v>
+      </c>
+      <c r="D30" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>1.3951694868629462E-2</v>
+      </c>
+      <c r="E30" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.7041044012282498</v>
+      </c>
+      <c r="F30" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
+        <v>45123.543749999997</v>
+      </c>
+      <c r="B31" s="8">
+        <v>2072078</v>
+      </c>
+      <c r="C31" s="8">
+        <v>14375</v>
+      </c>
+      <c r="D31" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>6.937480152774172E-3</v>
+      </c>
+      <c r="E31" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.85286591606960083</v>
+      </c>
+      <c r="F31" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
+        <v>45123.556250000001</v>
+      </c>
+      <c r="B32" s="8">
+        <v>2072078</v>
+      </c>
+      <c r="C32" s="8">
+        <v>14373</v>
+      </c>
+      <c r="D32" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>6.9365149381442207E-3</v>
+      </c>
+      <c r="E32" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.85288638689866936</v>
+      </c>
+      <c r="F32" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
+        <v>45123.561805555553</v>
+      </c>
+      <c r="B33" s="8">
+        <v>2072078</v>
+      </c>
+      <c r="C33" s="8">
+        <v>14372</v>
+      </c>
+      <c r="D33" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>6.936032330829245E-3</v>
+      </c>
+      <c r="E33" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.85289662231320373</v>
+      </c>
+      <c r="F33" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -1495,10 +1829,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D38BA54-A9BA-4382-B8C9-AD0F8112E2CF}">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1507,47 +1841,51 @@
     <col min="3" max="3" width="11.5546875" customWidth="1"/>
     <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C5">
         <v>1024</v>
@@ -1563,12 +1901,12 @@
         <v>45123</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C6">
         <v>512</v>
@@ -1584,12 +1922,12 @@
         <v>45123</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C7">
         <v>512</v>
@@ -1605,12 +1943,12 @@
         <v>45123</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="C8">
         <v>512</v>
@@ -1626,12 +1964,12 @@
         <v>45123</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C9">
         <v>2048</v>
@@ -1647,12 +1985,12 @@
         <v>45123</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B10" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C10" s="12">
         <v>16384</v>
@@ -1668,12 +2006,12 @@
         <v>45123</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C11" s="12">
         <v>8192</v>
@@ -1686,18 +2024,16 @@
         <v>376832</v>
       </c>
       <c r="F11" t="s">
-        <v>183</v>
-      </c>
-      <c r="G11" s="13">
-        <v>45123</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="C12" s="12">
         <v>16384</v>
@@ -1713,12 +2049,12 @@
         <v>45123</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="C13">
         <v>256</v>
@@ -1734,12 +2070,12 @@
         <v>45123</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="C14">
         <v>1024</v>
@@ -1752,12 +2088,12 @@
         <v>49152</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="C15">
         <v>1024</v>
@@ -1770,12 +2106,12 @@
         <v>6144</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C16">
         <v>1024</v>
@@ -1790,10 +2126,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C17" s="12">
         <v>65536</v>
@@ -1808,10 +2144,10 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C18">
         <v>512</v>
@@ -1826,10 +2162,10 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C19">
         <v>512</v>
@@ -1844,10 +2180,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C20">
         <v>256</v>
@@ -1862,10 +2198,10 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C21">
         <v>512</v>
@@ -1880,10 +2216,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C22">
         <v>512</v>
@@ -1898,10 +2234,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C23">
         <v>256</v>
@@ -1916,10 +2252,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C24">
         <v>512</v>
@@ -1934,10 +2270,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C25">
         <v>512</v>
@@ -1952,10 +2288,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C26">
         <v>256</v>
@@ -1970,10 +2306,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C27">
         <v>256</v>
@@ -1988,10 +2324,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C28">
         <v>256</v>
@@ -2006,10 +2342,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C29">
         <v>512</v>
@@ -2024,10 +2360,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C30">
         <v>512</v>
@@ -2042,10 +2378,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="C31">
         <v>256</v>
@@ -2060,10 +2396,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="C32">
         <v>1024</v>
@@ -2078,10 +2414,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B33" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="C33">
         <v>512</v>
@@ -2094,15 +2430,15 @@
         <v>3072</v>
       </c>
       <c r="F33" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B34" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="C34">
         <v>512</v>
@@ -2115,15 +2451,15 @@
         <v>3072</v>
       </c>
       <c r="F34" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C35">
         <v>512</v>
@@ -2136,15 +2472,15 @@
         <v>3072</v>
       </c>
       <c r="F35" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="C36">
         <v>512</v>
@@ -2157,15 +2493,15 @@
         <v>3072</v>
       </c>
       <c r="F36" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -2180,10 +2516,10 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -2198,10 +2534,10 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B39" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -2216,10 +2552,10 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B40" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="C40">
         <v>2</v>
@@ -2234,10 +2570,10 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B41" t="s">
-        <v>151</v>
+        <v>139</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -2252,10 +2588,10 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B42" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -2270,10 +2606,10 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -2288,10 +2624,10 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="C44">
         <v>2</v>
@@ -2306,10 +2642,10 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B45" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C45">
         <v>4</v>
@@ -2324,10 +2660,10 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B46" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="C46">
         <v>2</v>
@@ -2342,10 +2678,10 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B47" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C47">
         <v>2</v>
@@ -2360,10 +2696,10 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B48" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="C48">
         <v>8</v>
@@ -2376,12 +2712,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B49" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C49">
         <v>2</v>
@@ -2394,12 +2730,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="B50" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C50">
         <v>32</v>
@@ -2412,12 +2748,12 @@
         <v>512</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="B51" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="C51">
         <v>16</v>
@@ -2430,12 +2766,12 @@
         <v>256</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="B52" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="C52">
         <v>8</v>
@@ -2448,12 +2784,12 @@
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="B53" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="C53">
         <v>4</v>
@@ -2466,15 +2802,15 @@
         <v>32</v>
       </c>
       <c r="F53" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="B54" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="C54">
         <v>64</v>
@@ -2487,12 +2823,12 @@
         <v>3456</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="B55" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="C55">
         <v>128</v>
@@ -2505,15 +2841,15 @@
         <v>6912</v>
       </c>
       <c r="F55" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="C56">
         <v>2</v>
@@ -2526,12 +2862,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="B57" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C57">
         <v>2</v>
@@ -2544,12 +2880,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="B58" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="C58">
         <v>2</v>
@@ -2562,12 +2898,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="B59" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="C59">
         <v>2</v>
@@ -2580,12 +2916,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B60" t="s">
-        <v>170</v>
+        <v>158</v>
       </c>
       <c r="C60">
         <v>2</v>
@@ -2598,12 +2934,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B61" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="C61" s="12">
         <v>16384</v>
@@ -2616,12 +2952,12 @@
         <v>16384</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B62" t="s">
-        <v>172</v>
+        <v>160</v>
       </c>
       <c r="C62">
         <v>512</v>
@@ -2633,13 +2969,16 @@
         <f t="shared" si="0"/>
         <v>7168</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H62" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
       <c r="B63" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="C63">
         <v>1024</v>
@@ -2652,12 +2991,12 @@
         <v>6144</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="B64" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C64">
         <v>32</v>
@@ -2670,15 +3009,15 @@
         <v>416</v>
       </c>
       <c r="F64" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="B65" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="C65">
         <v>128</v>
@@ -2691,15 +3030,15 @@
         <v>6784</v>
       </c>
       <c r="F65" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="B66" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="C66">
         <v>128</v>
@@ -2714,10 +3053,10 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="B67" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="C67">
         <v>128</v>
@@ -2730,15 +3069,15 @@
         <v>1792</v>
       </c>
       <c r="G67" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B68" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="C68">
         <v>32</v>
@@ -2753,10 +3092,10 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="B69" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="C69">
         <v>16</v>
@@ -2771,10 +3110,10 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="B70" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="C70">
         <v>8</v>
@@ -2789,10 +3128,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B71" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C71">
         <v>4</v>
@@ -2807,7 +3146,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="E72" s="12">
         <f>SUBTOTAL(109,Table2[Total])</f>
@@ -2828,13 +3167,13 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.21875" customWidth="1"/>
+    <col min="3" max="3" width="50.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -2854,36 +3193,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>28</v>
+        <v>192</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>194</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>20</v>
+        <v>189</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>193</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>196</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -2892,18 +3231,18 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>195</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>37</v>
+        <v>182</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Fixed issues with multiple instructions Rotates did not set flags correctly EXX had register confusion problems
</commit_message>
<xml_diff>
--- a/test_files/validation/debug_book.xlsx
+++ b/test_files/validation/debug_book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Duncan Munro\Dropbox\dev\lazarus\computing\z80\box80\test_files\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6DD020-A2D3-4AC1-8495-3686367BD5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB84F142-C4E6-4E92-95D2-9BA9EA91BBA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="20076" windowHeight="11472" activeTab="1" xr2:uid="{84EB85F7-8048-4063-BC53-51767C72ED03}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="20076" windowHeight="11472" xr2:uid="{84EB85F7-8048-4063-BC53-51767C72ED03}"/>
   </bookViews>
   <sheets>
     <sheet name="Compliance" sheetId="2" r:id="rId1"/>
@@ -38,6 +38,40 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Duncan Munro</author>
+  </authors>
+  <commentList>
+    <comment ref="C37" authorId="0" shapeId="0" xr:uid="{C9BA8EC5-14CC-4D96-BE5B-2D0A92802083}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Duncan Munro:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+These are the remnants which are DAA, RLD, RRD instructions which differ between Z80 and Z180</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Duncan Munro</author>
@@ -72,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="203">
   <si>
     <t>Mem IY  IX  HL  DE  BC  F A SP</t>
   </si>
@@ -623,55 +657,64 @@
     <t>$00</t>
   </si>
   <si>
+    <t>_ _ _ _ _ _ _ _</t>
+  </si>
+  <si>
+    <t>SC131 tests re-run for &lt;rrd,rld&gt;</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Box80 is setting Z flag, Z180 isn't</t>
+  </si>
+  <si>
+    <t>Block move instructions had errors, now fixed</t>
+  </si>
+  <si>
+    <t>Box80 tests re-run for add iy,&lt;bc,de,iy,sp&gt;</t>
+  </si>
+  <si>
+    <t>Box80 tests re-run for bit n,(&lt;ix,iy&gt;+1)</t>
+  </si>
+  <si>
+    <t>Split CB DD xx 00-3F to avoid undocumented</t>
+  </si>
+  <si>
+    <t>Fixes to CB DD rotate instructions</t>
+  </si>
+  <si>
+    <t>Further fixes to CB DD rotate instructions</t>
+  </si>
+  <si>
+    <t>Added other rotate instructions CB</t>
+  </si>
+  <si>
+    <t>$ED $67</t>
+  </si>
+  <si>
+    <t>RRD</t>
+  </si>
+  <si>
+    <t>00918BC462FA030120E779B40006E28A</t>
+  </si>
+  <si>
+    <t>60918BC462FA030120E779B44400E28A</t>
+  </si>
+  <si>
+    <t>60918BC462FA030120E779B40400E28A</t>
+  </si>
+  <si>
     <t>$04</t>
   </si>
   <si>
-    <t>_ _ _ _ _ _ _ _</t>
+    <t>$44</t>
   </si>
   <si>
     <t>_ _ _ _ _ P _ _</t>
   </si>
   <si>
-    <t>SC131 tests re-run for &lt;rrd,rld&gt;</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Box80 is setting Z flag, Z180 isn't</t>
-  </si>
-  <si>
-    <t>$14</t>
-  </si>
-  <si>
-    <t>_ _ _ H _ P _ _</t>
-  </si>
-  <si>
-    <t>Block move instructions had errors, now fixed</t>
-  </si>
-  <si>
-    <t>$FD $09</t>
-  </si>
-  <si>
-    <t>ADD IY,BC</t>
-  </si>
-  <si>
-    <t>C2C72624C151963EF40F0F51921EEA71</t>
-  </si>
-  <si>
-    <t>C2C73575C151963EC7119EC151963EF4</t>
-  </si>
-  <si>
-    <t>C2C73575C151963EF40F0F51801EEA71</t>
-  </si>
-  <si>
-    <t>$2426 + $510F -&gt; $7535</t>
-  </si>
-  <si>
-    <t>Box80 tests re-run for add iy,&lt;bc,de,iy,sp&gt;</t>
-  </si>
-  <si>
-    <t>Box80 tests re-run for bit n,(&lt;ix,iy&gt;+1)</t>
+    <t>_ Z _ _ _ P _ _</t>
   </si>
 </sst>
 </file>
@@ -846,8 +889,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CCD46394-3C59-49D5-A3BE-54484FCE77F1}" name="Table1" displayName="Table1" ref="A6:F33" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A6:F33" xr:uid="{CCD46394-3C59-49D5-A3BE-54484FCE77F1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CCD46394-3C59-49D5-A3BE-54484FCE77F1}" name="Table1" displayName="Table1" ref="A6:F37" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A6:F37" xr:uid="{CCD46394-3C59-49D5-A3BE-54484FCE77F1}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{645467FE-6092-4669-8C66-53405E1B316C}" name="Date/Tim" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{0FDF52E0-80D4-44BC-BCD2-1F61AB42DBEC}" name="Tests     " dataDxfId="6" dataCellStyle="Comma"/>
@@ -1177,11 +1220,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D7535A-9EF6-43CB-A66F-D74C02DC0D46}">
-  <dimension ref="A1:F33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D7535A-9EF6-43CB-A66F-D74C02DC0D46}">
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1750,7 +1793,7 @@
         <v>0.7041044012282498</v>
       </c>
       <c r="F30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1772,7 +1815,7 @@
         <v>0.85286591606960083</v>
       </c>
       <c r="F31" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1794,7 +1837,7 @@
         <v>0.85288638689866936</v>
       </c>
       <c r="F32" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -1816,13 +1859,102 @@
         <v>0.85289662231320373</v>
       </c>
       <c r="F33" t="s">
-        <v>199</v>
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
+        <v>45123.765972222223</v>
+      </c>
+      <c r="B34" s="8">
+        <v>2237798</v>
+      </c>
+      <c r="C34" s="8">
+        <v>14757</v>
+      </c>
+      <c r="D34" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>6.5944289877817386E-3</v>
+      </c>
+      <c r="E34" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.84895598771750258</v>
+      </c>
+      <c r="F34" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
+        <v>45123.774305555555</v>
+      </c>
+      <c r="B35" s="8">
+        <v>2237798</v>
+      </c>
+      <c r="C35" s="8">
+        <v>14671</v>
+      </c>
+      <c r="D35" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>6.5559983519513382E-3</v>
+      </c>
+      <c r="E35" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.8498362333674514</v>
+      </c>
+      <c r="F35" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
+        <v>45123.78402777778</v>
+      </c>
+      <c r="B36" s="8">
+        <v>2237798</v>
+      </c>
+      <c r="C36" s="8">
+        <v>14372</v>
+      </c>
+      <c r="D36" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>6.4223848622619196E-3</v>
+      </c>
+      <c r="E36" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.85289662231320373</v>
+      </c>
+      <c r="F36" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
+        <v>45123.807638888888</v>
+      </c>
+      <c r="B37" s="8">
+        <v>2243839</v>
+      </c>
+      <c r="C37" s="8">
+        <v>14372</v>
+      </c>
+      <c r="D37" s="6">
+        <f>Table1[[#This Row],[Failures     ]]/Table1[[#This Row],[Tests     ]]</f>
+        <v>6.405094126628515E-3</v>
+      </c>
+      <c r="E37" s="10">
+        <f>($C$7-Table1[[#This Row],[Failures     ]])/$C$7</f>
+        <v>0.85289662231320373</v>
+      </c>
+      <c r="F37" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1831,7 +1963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D38BA54-A9BA-4382-B8C9-AD0F8112E2CF}">
   <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1877,7 +2009,7 @@
         <v>36</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -2970,7 +3102,7 @@
         <v>7168</v>
       </c>
       <c r="H62" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
@@ -3167,7 +3299,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3193,36 +3325,36 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -3231,19 +3363,17 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>184</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C6" s="1" t="s">
-        <v>197</v>
-      </c>
+      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C7" s="1"/>

</xml_diff>